<commit_message>
minor fixes, reset fuji contracts
</commit_message>
<xml_diff>
--- a/docs/faqs.xlsx
+++ b/docs/faqs.xlsx
@@ -5,16 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Github\sporteth0\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Github\sporteth\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506CE7C6-8A89-4B0B-93A7-5FC5950471E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C555E4-6BF2-4CD0-8E43-6B7207E6532A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2025" windowWidth="25875" windowHeight="11295" xr2:uid="{ED304670-DDB2-49C3-8B51-405BE1F15E00}"/>
+    <workbookView xWindow="1770" yWindow="2910" windowWidth="23940" windowHeight="11295" activeTab="1" xr2:uid="{ED304670-DDB2-49C3-8B51-405BE1F15E00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="gas" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="113">
   <si>
     <t>initialPost</t>
   </si>
@@ -210,9 +211,6 @@
     <t>Token</t>
   </si>
   <si>
-    <t>transferSpecial/Deposit</t>
-  </si>
-  <si>
     <t>Oracle</t>
   </si>
   <si>
@@ -237,27 +235,6 @@
     <t>0x9b4b402eA6eaE209Dc7741eb343D0dEDA17b6eE3</t>
   </si>
   <si>
-    <t>python</t>
-  </si>
-  <si>
-    <t>update</t>
-  </si>
-  <si>
-    <t>settle</t>
-  </si>
-  <si>
-    <t>init</t>
-  </si>
-  <si>
-    <t>process</t>
-  </si>
-  <si>
-    <t>VoteNo</t>
-  </si>
-  <si>
-    <t>VoteYes</t>
-  </si>
-  <si>
     <t>b'uxeQ~\xf2q\xa9o\xb397\xaa\xfe\x17\x12&amp;StR\x9a\xc4\xb3\x1a\xbb6Q\xb3\x84\xa5\x03\x91'</t>
   </si>
   <si>
@@ -277,20 +254,144 @@
   </si>
   <si>
     <t>0xd6F61ee5472dD41b6784AcDCAda6155871EFddaA</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Initial slate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday </t>
+  </si>
+  <si>
+    <t>settlement</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Tues</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>odds update</t>
+  </si>
+  <si>
+    <t>Friday*</t>
+  </si>
+  <si>
+    <t>Thursday*</t>
+  </si>
+  <si>
+    <t>Wednesday*</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>all times 12:00-13:00 GMT</t>
+  </si>
+  <si>
+    <t>12:00 GMT is 8:00 AM New York Time in summer</t>
+  </si>
+  <si>
+    <t>12:00 GMT is 7:00 AM New York Time in winter</t>
+  </si>
+  <si>
+    <t>0xEaFE27B34650ff68b085928541e567A9873216A9</t>
+  </si>
+  <si>
+    <t>0x55210ffc90fB44AE08983A1D87De7A9AdaE04BC1</t>
+  </si>
+  <si>
+    <t>0xB17452c78bdA4ddea7F3Da60BF381d6230a2Dbc6</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>send @ 12:00-13:00 GMT</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>betContracts</t>
+  </si>
+  <si>
+    <t>    uint32</t>
+  </si>
+  <si>
+    <t>    uint64</t>
+  </si>
+  <si>
+    <t>    addres</t>
+  </si>
+  <si>
+    <t>matchNum</t>
+  </si>
+  <si>
+    <t>pick</t>
+  </si>
+  <si>
+    <t>betAmount</t>
+  </si>
+  <si>
+    <t>payoff</t>
+  </si>
+  <si>
+    <t>s bettor</t>
+  </si>
+  <si>
+    <t>lasts from settlement to settlement</t>
+  </si>
+  <si>
+    <t>from  0 to 31</t>
+  </si>
+  <si>
+    <t>0 or 1</t>
+  </si>
+  <si>
+    <t>amount bet, 1e4 represents 1 avax</t>
+  </si>
+  <si>
+    <t>gross payout for bettor</t>
+  </si>
+  <si>
+    <t>bettor address</t>
+  </si>
+  <si>
+    <t>userStruct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0E+00;[Red]0E+00"/>
     <numFmt numFmtId="167" formatCode="0.0%;[Red]\-0.0%"/>
     <numFmt numFmtId="168" formatCode="0.00E+00;[Red]0.00E+00"/>
+    <numFmt numFmtId="169" formatCode="0.00%;[Red]\-0.00%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,18 +430,177 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -350,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -374,6 +634,51 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +996,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1622,7 @@
         <v>56</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L30">
         <f>L29/L28</f>
@@ -1326,23 +1631,23 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
         <v>63</v>
-      </c>
-      <c r="E31" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -1353,12 +1658,12 @@
     </row>
     <row r="36" spans="3:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D36" s="11" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="3:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="D37" s="11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -1366,7 +1671,7 @@
         <v>45157</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
@@ -1389,59 +1694,59 @@
         <v>56</v>
       </c>
       <c r="E42" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F42" t="s">
+        <v>58</v>
+      </c>
+      <c r="G42" t="s">
         <v>59</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>60</v>
       </c>
-      <c r="H42" t="s">
-        <v>61</v>
-      </c>
       <c r="I42" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E43" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F43" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" t="s">
         <v>59</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>60</v>
       </c>
-      <c r="H43" t="s">
-        <v>61</v>
-      </c>
       <c r="I43" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" t="s">
         <v>58</v>
       </c>
-      <c r="E44" t="s">
-        <v>79</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>59</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>60</v>
       </c>
-      <c r="H44" t="s">
-        <v>61</v>
-      </c>
       <c r="I44" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1451,65 +1756,1005 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0022EBE-CA85-42A1-BF2D-3D69939B3BC7}">
-  <dimension ref="E3:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52E05E7-B165-45C0-8B6B-813B2086E5D6}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="C3:X31"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="11" width="7.42578125" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" customWidth="1"/>
+    <col min="23" max="23" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
+    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F20" si="0">INT(G5/1000)*1000</f>
+        <v>410000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>410528</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5:L20" si="1">C$2*G5*D$2/1000000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>129000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>129535</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>112000</v>
+      </c>
+      <c r="G7" s="1">
+        <v>112165</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>72000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>72115</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8">
+        <f>2^8</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>99000</v>
+      </c>
+      <c r="G9" s="1">
+        <v>99820</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>241000</v>
+      </c>
+      <c r="G10" s="1">
+        <v>241935</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10">
+        <v>20</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>37000</v>
+      </c>
+      <c r="G11" s="1">
+        <v>37533</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>30</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>48</v>
+      </c>
+      <c r="W11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>52000</v>
+      </c>
+      <c r="G12" s="1">
+        <v>52578</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W12">
+        <f>24*365</f>
+        <v>8760</v>
+      </c>
+    </row>
+    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>84000</v>
+      </c>
+      <c r="G13" s="1">
+        <v>84469</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>142000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>142937</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>50</v>
+      </c>
+      <c r="W14" s="43">
+        <f>(1+W11)^W12</f>
+        <v>9.4341111137975214E+18</v>
+      </c>
+    </row>
+    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>54000</v>
+      </c>
+      <c r="G15" s="1">
+        <v>54888</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>51</v>
+      </c>
+      <c r="W15">
+        <f>1000000</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="16" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>48000</v>
+      </c>
+      <c r="G16" s="1">
+        <v>48120</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>15</v>
+      </c>
+      <c r="W16" s="5">
+        <f>W15*1000</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>44000</v>
+      </c>
+      <c r="G17" s="1">
+        <v>44945</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="W17" s="5">
+        <f>W16*1000</f>
+        <v>1000000000000</v>
+      </c>
+      <c r="X17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>33000</v>
+      </c>
+      <c r="G18" s="1">
+        <v>33637</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>53</v>
+      </c>
+      <c r="W18" s="5">
+        <f>W17*1000</f>
+        <v>1000000000000000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>62000</v>
+      </c>
+      <c r="G19" s="1">
+        <v>62228</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19">
+        <v>32</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>54</v>
+      </c>
+      <c r="W19" s="5">
+        <f>W18*1000</f>
+        <v>1E+18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>55000</v>
+      </c>
+      <c r="G20" s="1">
+        <v>55895</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>19</v>
+      </c>
+      <c r="O20">
+        <v>32</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O21">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="E22" s="7">
+        <v>100000000000000</v>
+      </c>
+      <c r="F22" s="1">
+        <f>1000000000000000000</f>
+        <v>1E+18</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="E23" s="7">
+        <v>5000000000000</v>
+      </c>
+      <c r="F23">
+        <f>0.05*F22</f>
+        <v>5E+16</v>
+      </c>
+      <c r="G23">
+        <f>F23/1000000000000000000</f>
+        <v>0.05</v>
+      </c>
+      <c r="P23" t="s">
+        <v>97</v>
+      </c>
+      <c r="T23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="P24" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>17</v>
+      </c>
+      <c r="R24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="P25" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>101</v>
+      </c>
+      <c r="R25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="P26" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>102</v>
+      </c>
+      <c r="R26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+      <c r="F27" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="P27" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>103</v>
+      </c>
+      <c r="R27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>104</v>
+      </c>
+      <c r="R28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="P29" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>105</v>
+      </c>
+      <c r="R29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="F31" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0022EBE-CA85-42A1-BF2D-3D69939B3BC7}">
+  <dimension ref="D3:K25"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
       <c r="E5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J5" s="43">
+        <v>1000000</v>
+      </c>
+      <c r="K5" s="5">
+        <f>J5*1000</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="44">
+        <f>0.002</f>
+        <v>2E-3</v>
+      </c>
+      <c r="J6">
+        <v>133333</v>
+      </c>
+      <c r="K6" s="5">
+        <f>J6*1000</f>
+        <v>133333000</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="1">
+        <f>J5*0.002</f>
+        <v>2000</v>
+      </c>
+      <c r="K7" s="5">
+        <f>J7*1000</f>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9">
+        <f>H6*H5</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="H10" s="5">
+        <f>H9*1000</f>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="26"/>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>